<commit_message>
Add 'tasks.xlsx' content Add new dashboard design
</commit_message>
<xml_diff>
--- a/doc/tasks.xlsx
+++ b/doc/tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\git\web\plan-it\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2476AB-645D-4AA8-A2E8-1C9CBF63C6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C77312-4906-4A3F-A583-522D85B4793D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="438" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="438" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Task</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -76,6 +76,34 @@
     <t>Pass</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>dark mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-&gt; tailwind</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Due -&gt; End in List pages</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>icon pack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>created at -&gt; added</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'created at' overwritten when modifying</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -86,7 +114,7 @@
     <numFmt numFmtId="176" formatCode="yy&quot;-&quot;m&quot;-&quot;d;@"/>
     <numFmt numFmtId="177" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="돋움"/>
@@ -102,14 +130,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="돋움"/>
-      <family val="3"/>
-      <charset val="129"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="9" tint="-0.499984740745262"/>
       <name val="돋움"/>
       <family val="3"/>
       <charset val="129"/>
@@ -137,11 +157,8 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -159,28 +176,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -191,6 +193,42 @@
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -559,635 +597,683 @@
   <dimension ref="A1:F165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="59.21875" style="2" customWidth="1"/>
-    <col min="3" max="4" width="11.5546875" style="13" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" style="14" customWidth="1"/>
-    <col min="6" max="6" width="50.21875" style="9" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="2.77734375" style="18" customWidth="1"/>
+    <col min="2" max="2" width="59.21875" style="16" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="22" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" style="22" customWidth="1"/>
+    <col min="6" max="6" width="50.21875" style="14" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="12"/>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="7"/>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="4"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="9"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="21">
+        <v>45777</v>
+      </c>
+      <c r="E2" s="21"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="13"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="22">
+        <v>45777</v>
+      </c>
     </row>
     <row r="4" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="9"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="21">
+        <v>45777</v>
+      </c>
+      <c r="E4" s="21"/>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="13"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="22">
+        <v>45777</v>
+      </c>
     </row>
     <row r="6" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="9"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="21">
+        <v>45777</v>
+      </c>
+      <c r="E6" s="21"/>
+      <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="9"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="4"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="9"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="9"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="9"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="13"/>
+      <c r="A11" s="15"/>
     </row>
     <row r="12" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="9"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="9"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="14"/>
     </row>
     <row r="14" spans="1:6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="9"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="14"/>
     </row>
     <row r="15" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="9"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="14"/>
     </row>
     <row r="16" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="9"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="14"/>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="13"/>
+      <c r="A17" s="15"/>
     </row>
     <row r="18" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="9"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="14"/>
     </row>
     <row r="19" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="9"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="14"/>
     </row>
     <row r="20" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="4"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="9"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="14"/>
     </row>
     <row r="21" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="9"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="14"/>
     </row>
     <row r="22" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="9"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="13"/>
+      <c r="A23" s="15"/>
     </row>
     <row r="24" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="4"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="9"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="14"/>
     </row>
     <row r="25" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="9"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="14"/>
     </row>
     <row r="26" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="9"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="14"/>
     </row>
     <row r="27" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="9"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="14"/>
     </row>
     <row r="28" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="9"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="14"/>
     </row>
     <row r="29" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="13"/>
+      <c r="A29" s="15"/>
     </row>
     <row r="30" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="13"/>
+      <c r="A30" s="15"/>
     </row>
     <row r="31" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="9"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="14"/>
     </row>
     <row r="32" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="9"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="14"/>
     </row>
     <row r="33" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="9"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="14"/>
     </row>
     <row r="34" spans="1:6" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="9"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="14"/>
     </row>
     <row r="35" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="13"/>
+      <c r="A35" s="15"/>
     </row>
     <row r="36" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="13"/>
+      <c r="A36" s="15"/>
     </row>
     <row r="37" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="13"/>
+      <c r="A37" s="15"/>
     </row>
     <row r="38" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="13"/>
+      <c r="A38" s="15"/>
     </row>
     <row r="39" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="13"/>
+      <c r="A39" s="15"/>
     </row>
     <row r="40" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="13"/>
+      <c r="A40" s="15"/>
     </row>
     <row r="41" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="13"/>
+      <c r="A41" s="15"/>
     </row>
     <row r="42" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="13"/>
+      <c r="A42" s="15"/>
     </row>
     <row r="43" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="13"/>
+      <c r="A43" s="15"/>
     </row>
     <row r="44" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="13"/>
+      <c r="A44" s="15"/>
     </row>
     <row r="45" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="13"/>
+      <c r="A45" s="15"/>
     </row>
     <row r="46" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="13"/>
+      <c r="A46" s="15"/>
     </row>
     <row r="47" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="13"/>
+      <c r="A47" s="15"/>
     </row>
     <row r="48" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="13"/>
+      <c r="A48" s="15"/>
     </row>
     <row r="49" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="13"/>
+      <c r="A49" s="15"/>
     </row>
     <row r="50" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="13"/>
+      <c r="A50" s="15"/>
     </row>
     <row r="51" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="13"/>
+      <c r="A51" s="15"/>
     </row>
     <row r="52" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="13"/>
+      <c r="A52" s="15"/>
     </row>
     <row r="53" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="13"/>
+      <c r="A53" s="15"/>
     </row>
     <row r="54" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="13"/>
+      <c r="A54" s="15"/>
     </row>
     <row r="55" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="13"/>
+      <c r="A55" s="15"/>
     </row>
     <row r="56" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="13"/>
+      <c r="A56" s="15"/>
     </row>
     <row r="57" spans="1:1" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="13"/>
+      <c r="A57" s="15"/>
     </row>
     <row r="58" spans="1:1" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="13"/>
+      <c r="A58" s="15"/>
     </row>
     <row r="59" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="13"/>
+      <c r="A59" s="15"/>
     </row>
     <row r="60" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="13"/>
+      <c r="A60" s="15"/>
     </row>
     <row r="61" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="13"/>
+      <c r="A61" s="15"/>
     </row>
     <row r="62" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="13"/>
+      <c r="A62" s="15"/>
     </row>
     <row r="63" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="13"/>
+      <c r="A63" s="15"/>
     </row>
     <row r="64" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="13"/>
+      <c r="A64" s="15"/>
     </row>
     <row r="65" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="13"/>
+      <c r="A65" s="15"/>
     </row>
     <row r="66" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="13"/>
+      <c r="A66" s="15"/>
     </row>
     <row r="67" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="13"/>
+      <c r="A67" s="15"/>
     </row>
     <row r="68" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="13"/>
+      <c r="A68" s="15"/>
     </row>
     <row r="69" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="13"/>
+      <c r="A69" s="15"/>
     </row>
     <row r="70" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="13"/>
+      <c r="A70" s="15"/>
     </row>
     <row r="71" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="13"/>
+      <c r="A71" s="15"/>
     </row>
     <row r="72" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="13"/>
+      <c r="A72" s="15"/>
     </row>
     <row r="73" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="13"/>
+      <c r="A73" s="15"/>
     </row>
     <row r="74" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="13"/>
+      <c r="A74" s="15"/>
     </row>
     <row r="75" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A75" s="13"/>
+      <c r="A75" s="15"/>
     </row>
     <row r="76" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="13"/>
+      <c r="A76" s="15"/>
     </row>
     <row r="77" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="13"/>
+      <c r="A77" s="15"/>
     </row>
     <row r="78" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="13"/>
+      <c r="A78" s="15"/>
     </row>
     <row r="79" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="13"/>
+      <c r="A79" s="15"/>
     </row>
     <row r="80" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A80" s="13"/>
+      <c r="A80" s="15"/>
     </row>
     <row r="81" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A81" s="13"/>
+      <c r="A81" s="15"/>
     </row>
     <row r="82" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A82" s="13"/>
+      <c r="A82" s="15"/>
     </row>
     <row r="83" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="13"/>
+      <c r="A83" s="15"/>
     </row>
     <row r="84" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="13"/>
+      <c r="A84" s="15"/>
     </row>
     <row r="85" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="13"/>
+      <c r="A85" s="15"/>
     </row>
     <row r="86" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A86" s="13"/>
+      <c r="A86" s="15"/>
     </row>
     <row r="87" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A87" s="13"/>
+      <c r="A87" s="15"/>
     </row>
     <row r="88" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="13"/>
+      <c r="A88" s="15"/>
     </row>
     <row r="89" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A89" s="13"/>
+      <c r="A89" s="15"/>
     </row>
     <row r="90" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A90" s="13"/>
+      <c r="A90" s="15"/>
     </row>
     <row r="91" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A91" s="13"/>
+      <c r="A91" s="15"/>
     </row>
     <row r="92" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A92" s="13"/>
+      <c r="A92" s="15"/>
     </row>
     <row r="93" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="13"/>
+      <c r="A93" s="15"/>
     </row>
     <row r="94" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A94" s="13"/>
+      <c r="A94" s="15"/>
     </row>
     <row r="95" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A95" s="13"/>
+      <c r="A95" s="15"/>
     </row>
     <row r="96" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A96" s="13"/>
+      <c r="A96" s="15"/>
     </row>
     <row r="97" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A97" s="13"/>
+      <c r="A97" s="15"/>
     </row>
     <row r="98" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="13"/>
+      <c r="A98" s="15"/>
     </row>
     <row r="99" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A99" s="13"/>
+      <c r="A99" s="15"/>
     </row>
     <row r="100" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A100" s="13"/>
+      <c r="A100" s="15"/>
     </row>
     <row r="101" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A101" s="13"/>
+      <c r="A101" s="15"/>
     </row>
     <row r="102" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A102" s="13"/>
+      <c r="A102" s="15"/>
     </row>
     <row r="103" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="13"/>
+      <c r="A103" s="15"/>
     </row>
     <row r="104" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A104" s="13"/>
+      <c r="A104" s="15"/>
     </row>
     <row r="105" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A105" s="13"/>
+      <c r="A105" s="15"/>
     </row>
     <row r="106" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A106" s="13"/>
+      <c r="A106" s="15"/>
     </row>
     <row r="107" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A107" s="13"/>
+      <c r="A107" s="15"/>
     </row>
     <row r="108" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A108" s="13"/>
+      <c r="A108" s="15"/>
     </row>
     <row r="109" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A109" s="13"/>
+      <c r="A109" s="15"/>
     </row>
     <row r="110" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A110" s="13"/>
+      <c r="A110" s="15"/>
     </row>
     <row r="111" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A111" s="13"/>
+      <c r="A111" s="15"/>
     </row>
     <row r="112" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A112" s="13"/>
+      <c r="A112" s="15"/>
     </row>
     <row r="113" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A113" s="13"/>
+      <c r="A113" s="15"/>
     </row>
     <row r="114" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A114" s="13"/>
+      <c r="A114" s="15"/>
     </row>
     <row r="115" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A115" s="13"/>
+      <c r="A115" s="15"/>
     </row>
     <row r="116" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A116" s="13"/>
+      <c r="A116" s="15"/>
     </row>
     <row r="117" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A117" s="13"/>
+      <c r="A117" s="15"/>
     </row>
     <row r="118" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A118" s="13"/>
+      <c r="A118" s="15"/>
     </row>
     <row r="119" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A119" s="13"/>
+      <c r="A119" s="15"/>
     </row>
     <row r="120" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A120" s="13"/>
+      <c r="A120" s="15"/>
     </row>
     <row r="121" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A121" s="13"/>
+      <c r="A121" s="15"/>
     </row>
     <row r="122" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A122" s="13"/>
+      <c r="A122" s="15"/>
     </row>
     <row r="123" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A123" s="13"/>
+      <c r="A123" s="15"/>
     </row>
     <row r="124" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A124" s="13"/>
+      <c r="A124" s="15"/>
     </row>
     <row r="125" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A125" s="13"/>
+      <c r="A125" s="15"/>
     </row>
     <row r="126" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A126" s="13"/>
+      <c r="A126" s="15"/>
     </row>
     <row r="127" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A127" s="13"/>
+      <c r="A127" s="15"/>
     </row>
     <row r="128" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A128" s="13"/>
+      <c r="A128" s="15"/>
     </row>
     <row r="129" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A129" s="13"/>
+      <c r="A129" s="15"/>
     </row>
     <row r="130" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A130" s="13"/>
+      <c r="A130" s="15"/>
     </row>
     <row r="131" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A131" s="13"/>
+      <c r="A131" s="15"/>
     </row>
     <row r="132" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A132" s="13"/>
+      <c r="A132" s="15"/>
     </row>
     <row r="133" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A133" s="13"/>
+      <c r="A133" s="15"/>
     </row>
     <row r="134" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A134" s="13"/>
+      <c r="A134" s="15"/>
     </row>
     <row r="135" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A135" s="13"/>
+      <c r="A135" s="15"/>
     </row>
     <row r="136" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A136" s="13"/>
+      <c r="A136" s="15"/>
     </row>
     <row r="137" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A137" s="13"/>
+      <c r="A137" s="15"/>
     </row>
     <row r="138" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A138" s="13"/>
+      <c r="A138" s="15"/>
     </row>
     <row r="139" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A139" s="13"/>
+      <c r="A139" s="15"/>
     </row>
     <row r="140" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A140" s="13"/>
+      <c r="A140" s="15"/>
     </row>
     <row r="141" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A141" s="13"/>
+      <c r="A141" s="15"/>
     </row>
     <row r="142" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A142" s="13"/>
+      <c r="A142" s="15"/>
     </row>
     <row r="143" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A143" s="13"/>
+      <c r="A143" s="15"/>
     </row>
     <row r="144" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A144" s="13"/>
+      <c r="A144" s="15"/>
     </row>
     <row r="145" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A145" s="13"/>
+      <c r="A145" s="15"/>
     </row>
     <row r="146" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A146" s="13"/>
+      <c r="A146" s="15"/>
     </row>
     <row r="147" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A147" s="13"/>
+      <c r="A147" s="15"/>
     </row>
     <row r="148" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A148" s="13"/>
+      <c r="A148" s="15"/>
     </row>
     <row r="149" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A149" s="13"/>
+      <c r="A149" s="15"/>
     </row>
     <row r="150" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A150" s="13"/>
+      <c r="A150" s="15"/>
     </row>
     <row r="151" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A151" s="13"/>
+      <c r="A151" s="15"/>
     </row>
     <row r="152" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A152" s="13"/>
+      <c r="A152" s="15"/>
     </row>
     <row r="153" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A153" s="13"/>
+      <c r="A153" s="15"/>
     </row>
     <row r="154" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A154" s="13"/>
+      <c r="A154" s="15"/>
     </row>
     <row r="155" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A155" s="13"/>
+      <c r="A155" s="15"/>
     </row>
     <row r="156" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A156" s="13"/>
+      <c r="A156" s="15"/>
     </row>
     <row r="157" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A157" s="13"/>
+      <c r="A157" s="15"/>
     </row>
     <row r="158" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A158" s="13"/>
+      <c r="A158" s="15"/>
     </row>
     <row r="159" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A159" s="13"/>
+      <c r="A159" s="15"/>
     </row>
     <row r="160" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A160" s="13"/>
+      <c r="A160" s="15"/>
     </row>
     <row r="161" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A161" s="13"/>
+      <c r="A161" s="15"/>
     </row>
     <row r="162" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A162" s="13"/>
+      <c r="A162" s="15"/>
     </row>
     <row r="163" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A163" s="13"/>
+      <c r="A163" s="15"/>
     </row>
     <row r="164" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A164" s="13"/>
+      <c r="A164" s="15"/>
     </row>
     <row r="165" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A165" s="13"/>
+      <c r="A165" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="B1:F69" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
@@ -1202,635 +1288,649 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F167"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="59.21875" style="2" customWidth="1"/>
-    <col min="3" max="4" width="11.5546875" style="13" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" style="14" customWidth="1"/>
-    <col min="6" max="6" width="50.21875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="1.6640625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="59.21875" style="16" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="22" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" style="22" customWidth="1"/>
+    <col min="6" max="6" width="50.21875" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="3"/>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="4"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="7"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="21">
+        <v>45777</v>
+      </c>
+      <c r="E2" s="21"/>
     </row>
     <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="4"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="21">
+        <v>45777</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="4"/>
-      <c r="B4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="7"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
     </row>
     <row r="5" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="4"/>
+      <c r="A5" s="12"/>
     </row>
     <row r="6" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="4"/>
-      <c r="B6"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="7"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
     </row>
     <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="4"/>
-      <c r="B7"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="7"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
     </row>
     <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="7"/>
+      <c r="A8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
     </row>
     <row r="9" spans="1:6" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A9" s="4"/>
-      <c r="B9"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="7"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
     </row>
     <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="4"/>
-      <c r="B10"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="7"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
     </row>
     <row r="11" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="4"/>
+      <c r="A11" s="12"/>
     </row>
     <row r="12" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="4"/>
-      <c r="B12"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="7"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
     </row>
     <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="4"/>
-      <c r="B13"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="7"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="4"/>
-      <c r="B14"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="7"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
     </row>
     <row r="15" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="4"/>
-      <c r="B15"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="7"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
     </row>
     <row r="16" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="4"/>
-      <c r="B16"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="7"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
     </row>
     <row r="17" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="4"/>
+      <c r="A17" s="12"/>
     </row>
     <row r="18" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="4"/>
-      <c r="B18"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="7"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
     </row>
     <row r="19" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="4"/>
-      <c r="B19"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="7"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
     </row>
     <row r="20" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="4"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="7"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
     </row>
     <row r="21" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="4"/>
-      <c r="B21"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="7"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
     </row>
     <row r="22" spans="1:5" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A22" s="4"/>
-      <c r="B22"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="7"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
     </row>
     <row r="23" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="4"/>
+      <c r="A23" s="12"/>
     </row>
     <row r="24" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="4"/>
-      <c r="B24"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="7"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
     </row>
     <row r="25" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="4"/>
-      <c r="B25"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="7"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
     </row>
     <row r="26" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="4"/>
-      <c r="B26"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="7"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
     </row>
     <row r="27" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="4"/>
-      <c r="B27"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="7"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
     </row>
     <row r="28" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="4"/>
-      <c r="B28"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="7"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
     </row>
     <row r="29" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="4"/>
+      <c r="A29" s="12"/>
     </row>
     <row r="30" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="4"/>
+      <c r="A30" s="12"/>
     </row>
     <row r="31" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="4"/>
-      <c r="B31"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="7"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
     </row>
     <row r="32" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="4"/>
-      <c r="B32"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="7"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
     </row>
     <row r="33" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="4"/>
-      <c r="B33"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="7"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
     </row>
     <row r="34" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="4"/>
-      <c r="B34"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="7"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
     </row>
     <row r="35" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="4"/>
+      <c r="A35" s="12"/>
     </row>
     <row r="36" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="4"/>
+      <c r="A36" s="12"/>
     </row>
     <row r="37" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="4"/>
+      <c r="A37" s="12"/>
     </row>
     <row r="38" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="4"/>
+      <c r="A38" s="12"/>
     </row>
     <row r="39" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="4"/>
+      <c r="A39" s="12"/>
     </row>
     <row r="40" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="4"/>
+      <c r="A40" s="12"/>
     </row>
     <row r="41" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="4"/>
+      <c r="A41" s="12"/>
     </row>
     <row r="42" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="4"/>
+      <c r="A42" s="12"/>
     </row>
     <row r="43" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="4"/>
+      <c r="A43" s="12"/>
     </row>
     <row r="44" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="4"/>
+      <c r="A44" s="12"/>
     </row>
     <row r="45" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="4"/>
+      <c r="A45" s="12"/>
     </row>
     <row r="46" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="4"/>
+      <c r="A46" s="12"/>
     </row>
     <row r="47" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="4"/>
+      <c r="A47" s="12"/>
     </row>
     <row r="48" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="4"/>
+      <c r="A48" s="12"/>
     </row>
     <row r="49" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="4"/>
+      <c r="A49" s="12"/>
     </row>
     <row r="50" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="4"/>
+      <c r="A50" s="12"/>
     </row>
     <row r="51" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="4"/>
+      <c r="A51" s="12"/>
     </row>
     <row r="52" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="4"/>
+      <c r="A52" s="12"/>
     </row>
     <row r="53" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="4"/>
+      <c r="A53" s="12"/>
     </row>
     <row r="54" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="4"/>
+      <c r="A54" s="12"/>
     </row>
     <row r="55" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="4"/>
+      <c r="A55" s="12"/>
     </row>
     <row r="56" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="4"/>
+      <c r="A56" s="12"/>
     </row>
     <row r="57" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="4"/>
+      <c r="A57" s="12"/>
     </row>
     <row r="58" spans="1:1" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A58" s="4"/>
+      <c r="A58" s="12"/>
     </row>
     <row r="59" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="4"/>
+      <c r="A59" s="12"/>
     </row>
     <row r="60" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="4"/>
+      <c r="A60" s="12"/>
     </row>
     <row r="61" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="4"/>
+      <c r="A61" s="12"/>
     </row>
     <row r="62" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="4"/>
+      <c r="A62" s="12"/>
     </row>
     <row r="63" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="4"/>
+      <c r="A63" s="12"/>
     </row>
     <row r="64" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="4"/>
+      <c r="A64" s="12"/>
     </row>
     <row r="65" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="4"/>
+      <c r="A65" s="12"/>
     </row>
     <row r="66" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="4"/>
+      <c r="A66" s="12"/>
     </row>
     <row r="67" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="4"/>
+      <c r="A67" s="12"/>
     </row>
     <row r="68" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="4"/>
+      <c r="A68" s="12"/>
     </row>
     <row r="69" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="4"/>
+      <c r="A69" s="12"/>
     </row>
     <row r="70" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="4"/>
+      <c r="A70" s="12"/>
     </row>
     <row r="71" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="4"/>
+      <c r="A71" s="12"/>
     </row>
     <row r="72" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="4"/>
+      <c r="A72" s="12"/>
     </row>
     <row r="73" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="4"/>
+      <c r="A73" s="12"/>
     </row>
     <row r="74" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="4"/>
+      <c r="A74" s="12"/>
     </row>
     <row r="75" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A75" s="4"/>
+      <c r="A75" s="12"/>
     </row>
     <row r="76" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="4"/>
+      <c r="A76" s="12"/>
     </row>
     <row r="77" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="4"/>
+      <c r="A77" s="12"/>
     </row>
     <row r="78" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="4"/>
+      <c r="A78" s="12"/>
     </row>
     <row r="79" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="4"/>
+      <c r="A79" s="12"/>
     </row>
     <row r="80" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A80" s="4"/>
+      <c r="A80" s="12"/>
     </row>
     <row r="81" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A81" s="4"/>
+      <c r="A81" s="12"/>
     </row>
     <row r="82" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A82" s="4"/>
+      <c r="A82" s="12"/>
     </row>
     <row r="83" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="4"/>
+      <c r="A83" s="12"/>
     </row>
     <row r="84" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="4"/>
+      <c r="A84" s="12"/>
     </row>
     <row r="85" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="4"/>
+      <c r="A85" s="12"/>
     </row>
     <row r="86" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A86" s="4"/>
+      <c r="A86" s="12"/>
     </row>
     <row r="87" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A87" s="4"/>
+      <c r="A87" s="12"/>
     </row>
     <row r="88" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="4"/>
+      <c r="A88" s="12"/>
     </row>
     <row r="89" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A89" s="4"/>
+      <c r="A89" s="12"/>
     </row>
     <row r="90" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A90" s="4"/>
+      <c r="A90" s="12"/>
     </row>
     <row r="91" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A91" s="4"/>
+      <c r="A91" s="12"/>
     </row>
     <row r="92" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A92" s="4"/>
+      <c r="A92" s="12"/>
     </row>
     <row r="93" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="4"/>
+      <c r="A93" s="12"/>
     </row>
     <row r="94" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A94" s="4"/>
+      <c r="A94" s="12"/>
     </row>
     <row r="95" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A95" s="4"/>
+      <c r="A95" s="12"/>
     </row>
     <row r="96" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A96" s="4"/>
+      <c r="A96" s="12"/>
     </row>
     <row r="97" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A97" s="4"/>
+      <c r="A97" s="12"/>
     </row>
     <row r="98" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="4"/>
+      <c r="A98" s="12"/>
     </row>
     <row r="99" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A99" s="4"/>
+      <c r="A99" s="12"/>
     </row>
     <row r="100" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A100" s="4"/>
+      <c r="A100" s="12"/>
     </row>
     <row r="101" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A101" s="4"/>
+      <c r="A101" s="12"/>
     </row>
     <row r="102" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A102" s="4"/>
+      <c r="A102" s="12"/>
     </row>
     <row r="103" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="4"/>
+      <c r="A103" s="12"/>
     </row>
     <row r="104" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A104" s="4"/>
+      <c r="A104" s="12"/>
     </row>
     <row r="105" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A105" s="4"/>
+      <c r="A105" s="12"/>
     </row>
     <row r="106" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A106" s="4"/>
+      <c r="A106" s="12"/>
     </row>
     <row r="107" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A107" s="4"/>
+      <c r="A107" s="12"/>
     </row>
     <row r="108" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A108" s="4"/>
+      <c r="A108" s="12"/>
     </row>
     <row r="109" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A109" s="4"/>
+      <c r="A109" s="12"/>
     </row>
     <row r="110" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A110" s="4"/>
+      <c r="A110" s="12"/>
     </row>
     <row r="111" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A111" s="4"/>
+      <c r="A111" s="12"/>
     </row>
     <row r="112" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A112" s="4"/>
+      <c r="A112" s="12"/>
     </row>
     <row r="113" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A113" s="4"/>
+      <c r="A113" s="12"/>
     </row>
     <row r="114" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A114" s="4"/>
+      <c r="A114" s="12"/>
     </row>
     <row r="115" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A115" s="4"/>
+      <c r="A115" s="12"/>
     </row>
     <row r="116" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A116" s="4"/>
+      <c r="A116" s="12"/>
     </row>
     <row r="117" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A117" s="4"/>
+      <c r="A117" s="12"/>
     </row>
     <row r="118" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A118" s="4"/>
+      <c r="A118" s="12"/>
     </row>
     <row r="119" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A119" s="4"/>
+      <c r="A119" s="12"/>
     </row>
     <row r="120" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A120" s="4"/>
+      <c r="A120" s="12"/>
     </row>
     <row r="121" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A121" s="4"/>
+      <c r="A121" s="12"/>
     </row>
     <row r="122" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A122" s="4"/>
+      <c r="A122" s="12"/>
     </row>
     <row r="123" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A123" s="4"/>
+      <c r="A123" s="12"/>
     </row>
     <row r="124" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A124" s="4"/>
+      <c r="A124" s="12"/>
     </row>
     <row r="125" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A125" s="4"/>
+      <c r="A125" s="12"/>
     </row>
     <row r="126" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A126" s="4"/>
+      <c r="A126" s="12"/>
     </row>
     <row r="127" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A127" s="4"/>
+      <c r="A127" s="12"/>
     </row>
     <row r="128" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A128" s="4"/>
+      <c r="A128" s="12"/>
     </row>
     <row r="129" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A129" s="4"/>
+      <c r="A129" s="12"/>
     </row>
     <row r="130" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A130" s="4"/>
+      <c r="A130" s="12"/>
     </row>
     <row r="131" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A131" s="4"/>
+      <c r="A131" s="12"/>
     </row>
     <row r="132" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A132" s="4"/>
+      <c r="A132" s="12"/>
     </row>
     <row r="133" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A133" s="4"/>
+      <c r="A133" s="12"/>
     </row>
     <row r="134" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A134" s="4"/>
+      <c r="A134" s="12"/>
     </row>
     <row r="135" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A135" s="4"/>
+      <c r="A135" s="12"/>
     </row>
     <row r="136" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A136" s="4"/>
+      <c r="A136" s="12"/>
     </row>
     <row r="137" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A137" s="4"/>
+      <c r="A137" s="12"/>
     </row>
     <row r="138" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A138" s="4"/>
+      <c r="A138" s="12"/>
     </row>
     <row r="139" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A139" s="4"/>
+      <c r="A139" s="12"/>
     </row>
     <row r="140" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A140" s="4"/>
+      <c r="A140" s="12"/>
     </row>
     <row r="141" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A141" s="4"/>
+      <c r="A141" s="12"/>
     </row>
     <row r="142" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A142" s="4"/>
+      <c r="A142" s="12"/>
     </row>
     <row r="143" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A143" s="4"/>
+      <c r="A143" s="12"/>
     </row>
     <row r="144" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A144" s="4"/>
+      <c r="A144" s="12"/>
     </row>
     <row r="145" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A145" s="4"/>
+      <c r="A145" s="12"/>
     </row>
     <row r="146" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A146" s="4"/>
+      <c r="A146" s="12"/>
     </row>
     <row r="147" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A147" s="4"/>
+      <c r="A147" s="12"/>
     </row>
     <row r="148" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A148" s="4"/>
+      <c r="A148" s="12"/>
     </row>
     <row r="149" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A149" s="4"/>
+      <c r="A149" s="12"/>
     </row>
     <row r="150" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A150" s="4"/>
+      <c r="A150" s="12"/>
     </row>
     <row r="151" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A151" s="4"/>
+      <c r="A151" s="12"/>
     </row>
     <row r="152" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A152" s="4"/>
+      <c r="A152" s="12"/>
     </row>
     <row r="153" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A153" s="4"/>
+      <c r="A153" s="12"/>
     </row>
     <row r="154" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A154" s="4"/>
+      <c r="A154" s="12"/>
     </row>
     <row r="155" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A155" s="4"/>
+      <c r="A155" s="12"/>
     </row>
     <row r="156" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A156" s="4"/>
+      <c r="A156" s="12"/>
     </row>
     <row r="157" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A157" s="4"/>
+      <c r="A157" s="12"/>
     </row>
     <row r="158" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A158" s="4"/>
+      <c r="A158" s="12"/>
     </row>
     <row r="159" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A159" s="4"/>
+      <c r="A159" s="12"/>
     </row>
     <row r="160" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A160" s="4"/>
+      <c r="A160" s="12"/>
     </row>
     <row r="161" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A161" s="4"/>
+      <c r="A161" s="12"/>
     </row>
     <row r="162" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A162" s="4"/>
+      <c r="A162" s="12"/>
     </row>
     <row r="163" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A163" s="4"/>
+      <c r="A163" s="12"/>
     </row>
     <row r="164" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A164" s="4"/>
+      <c r="A164" s="12"/>
     </row>
     <row r="165" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A165" s="4"/>
+      <c r="A165" s="12"/>
     </row>
     <row r="166" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A166" s="4"/>
+      <c r="A166" s="12"/>
     </row>
     <row r="167" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A167" s="4"/>
+      <c r="A167" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="B1:E34" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
@@ -1848,19 +1948,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="55.5546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="44.21875" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="55.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="44.21875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A1" s="16"/>
+      <c r="A1" s="10"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A8" s="16"/>
+      <c r="A8" s="10"/>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A14" s="16"/>
+      <c r="A14" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1873,526 +1973,526 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="43.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" style="17" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="13"/>
-    <col min="5" max="5" width="43.6640625" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="2.77734375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="8"/>
+    <col min="5" max="5" width="43.6640625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" s="12"/>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="7"/>
+      <c r="B1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="4"/>
+      <c r="A2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="13"/>
+      <c r="A3" s="8"/>
     </row>
     <row r="4" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="4"/>
+      <c r="A4" s="3"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="13"/>
+      <c r="A5" s="8"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="4"/>
+      <c r="A6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="4"/>
+      <c r="A7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="4"/>
+      <c r="A8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="4"/>
+      <c r="A9" s="3"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="4"/>
+      <c r="A10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="13"/>
+      <c r="A11" s="8"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="4"/>
+      <c r="A12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="4"/>
+      <c r="A13" s="3"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="4"/>
+      <c r="A14" s="3"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="4"/>
+      <c r="A15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="4"/>
+      <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A17" s="13"/>
+      <c r="A17" s="8"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A18" s="4"/>
+      <c r="A18" s="3"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A19" s="4"/>
+      <c r="A19" s="3"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A20" s="4"/>
+      <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A21" s="4"/>
+      <c r="A21" s="3"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A22" s="4"/>
+      <c r="A22" s="3"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A23" s="13"/>
+      <c r="A23" s="8"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A24" s="4"/>
+      <c r="A24" s="3"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A25" s="4"/>
+      <c r="A25" s="3"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A26" s="4"/>
+      <c r="A26" s="3"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A27" s="4"/>
+      <c r="A27" s="3"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A28" s="4"/>
+      <c r="A28" s="3"/>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A29" s="13"/>
+      <c r="A29" s="8"/>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A30" s="13"/>
+      <c r="A30" s="8"/>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A31" s="4"/>
+      <c r="A31" s="3"/>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A32" s="4"/>
+      <c r="A32" s="3"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A33" s="4"/>
+      <c r="A33" s="3"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A34" s="4"/>
+      <c r="A34" s="3"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A35" s="13"/>
+      <c r="A35" s="8"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A36" s="13"/>
+      <c r="A36" s="8"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A37" s="13"/>
+      <c r="A37" s="8"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A38" s="13"/>
+      <c r="A38" s="8"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A39" s="13"/>
+      <c r="A39" s="8"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A40" s="13"/>
+      <c r="A40" s="8"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A41" s="13"/>
+      <c r="A41" s="8"/>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A42" s="13"/>
+      <c r="A42" s="8"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A43" s="13"/>
+      <c r="A43" s="8"/>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A44" s="13"/>
+      <c r="A44" s="8"/>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A45" s="13"/>
+      <c r="A45" s="8"/>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A46" s="13"/>
+      <c r="A46" s="8"/>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A47" s="13"/>
+      <c r="A47" s="8"/>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A48" s="13"/>
+      <c r="A48" s="8"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A49" s="13"/>
+      <c r="A49" s="8"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A50" s="13"/>
+      <c r="A50" s="8"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A51" s="13"/>
+      <c r="A51" s="8"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A52" s="13"/>
+      <c r="A52" s="8"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A53" s="13"/>
+      <c r="A53" s="8"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A54" s="13"/>
+      <c r="A54" s="8"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A55" s="13"/>
+      <c r="A55" s="8"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A56" s="13"/>
+      <c r="A56" s="8"/>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A57" s="13"/>
+      <c r="A57" s="8"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A58" s="13"/>
+      <c r="A58" s="8"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A59" s="13"/>
+      <c r="A59" s="8"/>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A60" s="13"/>
+      <c r="A60" s="8"/>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A61" s="13"/>
+      <c r="A61" s="8"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A62" s="13"/>
+      <c r="A62" s="8"/>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A63" s="13"/>
+      <c r="A63" s="8"/>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A64" s="13"/>
+      <c r="A64" s="8"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A65" s="13"/>
+      <c r="A65" s="8"/>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A66" s="13"/>
+      <c r="A66" s="8"/>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A67" s="13"/>
+      <c r="A67" s="8"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A68" s="13"/>
+      <c r="A68" s="8"/>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A69" s="13"/>
+      <c r="A69" s="8"/>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A70" s="13"/>
+      <c r="A70" s="8"/>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A71" s="13"/>
+      <c r="A71" s="8"/>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A72" s="13"/>
+      <c r="A72" s="8"/>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A73" s="13"/>
+      <c r="A73" s="8"/>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A74" s="13"/>
+      <c r="A74" s="8"/>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A75" s="13"/>
+      <c r="A75" s="8"/>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A76" s="13"/>
+      <c r="A76" s="8"/>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A77" s="13"/>
+      <c r="A77" s="8"/>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A78" s="13"/>
+      <c r="A78" s="8"/>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A79" s="13"/>
+      <c r="A79" s="8"/>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A80" s="13"/>
+      <c r="A80" s="8"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A81" s="13"/>
+      <c r="A81" s="8"/>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A82" s="13"/>
+      <c r="A82" s="8"/>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A83" s="13"/>
+      <c r="A83" s="8"/>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A84" s="13"/>
+      <c r="A84" s="8"/>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A85" s="13"/>
+      <c r="A85" s="8"/>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A86" s="13"/>
+      <c r="A86" s="8"/>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A87" s="13"/>
+      <c r="A87" s="8"/>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A88" s="13"/>
+      <c r="A88" s="8"/>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A89" s="13"/>
+      <c r="A89" s="8"/>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A90" s="13"/>
+      <c r="A90" s="8"/>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A91" s="13"/>
+      <c r="A91" s="8"/>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A92" s="13"/>
+      <c r="A92" s="8"/>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A93" s="13"/>
+      <c r="A93" s="8"/>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A94" s="13"/>
+      <c r="A94" s="8"/>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A95" s="13"/>
+      <c r="A95" s="8"/>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A96" s="13"/>
+      <c r="A96" s="8"/>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A97" s="13"/>
+      <c r="A97" s="8"/>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A98" s="13"/>
+      <c r="A98" s="8"/>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A99" s="13"/>
+      <c r="A99" s="8"/>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A100" s="13"/>
+      <c r="A100" s="8"/>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A101" s="13"/>
+      <c r="A101" s="8"/>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A102" s="13"/>
+      <c r="A102" s="8"/>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A103" s="13"/>
+      <c r="A103" s="8"/>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A104" s="13"/>
+      <c r="A104" s="8"/>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A105" s="13"/>
+      <c r="A105" s="8"/>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A106" s="13"/>
+      <c r="A106" s="8"/>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A107" s="13"/>
+      <c r="A107" s="8"/>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A108" s="13"/>
+      <c r="A108" s="8"/>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A109" s="13"/>
+      <c r="A109" s="8"/>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A110" s="13"/>
+      <c r="A110" s="8"/>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A111" s="13"/>
+      <c r="A111" s="8"/>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A112" s="13"/>
+      <c r="A112" s="8"/>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A113" s="13"/>
+      <c r="A113" s="8"/>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A114" s="13"/>
+      <c r="A114" s="8"/>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A115" s="13"/>
+      <c r="A115" s="8"/>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A116" s="13"/>
+      <c r="A116" s="8"/>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A117" s="13"/>
+      <c r="A117" s="8"/>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A118" s="13"/>
+      <c r="A118" s="8"/>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A119" s="13"/>
+      <c r="A119" s="8"/>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A120" s="13"/>
+      <c r="A120" s="8"/>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A121" s="13"/>
+      <c r="A121" s="8"/>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A122" s="13"/>
+      <c r="A122" s="8"/>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A123" s="13"/>
+      <c r="A123" s="8"/>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A124" s="13"/>
+      <c r="A124" s="8"/>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A125" s="13"/>
+      <c r="A125" s="8"/>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A126" s="13"/>
+      <c r="A126" s="8"/>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A127" s="13"/>
+      <c r="A127" s="8"/>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A128" s="13"/>
+      <c r="A128" s="8"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A129" s="13"/>
+      <c r="A129" s="8"/>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A130" s="13"/>
+      <c r="A130" s="8"/>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A131" s="13"/>
+      <c r="A131" s="8"/>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A132" s="13"/>
+      <c r="A132" s="8"/>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A133" s="13"/>
+      <c r="A133" s="8"/>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A134" s="13"/>
+      <c r="A134" s="8"/>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A135" s="13"/>
+      <c r="A135" s="8"/>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A136" s="13"/>
+      <c r="A136" s="8"/>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A137" s="13"/>
+      <c r="A137" s="8"/>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A138" s="13"/>
+      <c r="A138" s="8"/>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A139" s="13"/>
+      <c r="A139" s="8"/>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A140" s="13"/>
+      <c r="A140" s="8"/>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A141" s="13"/>
+      <c r="A141" s="8"/>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A142" s="13"/>
+      <c r="A142" s="8"/>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A143" s="13"/>
+      <c r="A143" s="8"/>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A144" s="13"/>
+      <c r="A144" s="8"/>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A145" s="13"/>
+      <c r="A145" s="8"/>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A146" s="13"/>
+      <c r="A146" s="8"/>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A147" s="13"/>
+      <c r="A147" s="8"/>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A148" s="13"/>
+      <c r="A148" s="8"/>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A149" s="13"/>
+      <c r="A149" s="8"/>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A150" s="13"/>
+      <c r="A150" s="8"/>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A151" s="13"/>
+      <c r="A151" s="8"/>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A152" s="13"/>
+      <c r="A152" s="8"/>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A153" s="13"/>
+      <c r="A153" s="8"/>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A154" s="13"/>
+      <c r="A154" s="8"/>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A155" s="13"/>
+      <c r="A155" s="8"/>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A156" s="13"/>
+      <c r="A156" s="8"/>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A157" s="13"/>
+      <c r="A157" s="8"/>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A158" s="13"/>
+      <c r="A158" s="8"/>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A159" s="13"/>
+      <c r="A159" s="8"/>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A160" s="13"/>
+      <c r="A160" s="8"/>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A161" s="13"/>
+      <c r="A161" s="8"/>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A162" s="13"/>
+      <c r="A162" s="8"/>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A163" s="13"/>
+      <c r="A163" s="8"/>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A164" s="13"/>
+      <c r="A164" s="8"/>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A165" s="13"/>
+      <c r="A165" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
update list table headers
</commit_message>
<xml_diff>
--- a/doc/tasks.xlsx
+++ b/doc/tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\git\web\plan-it\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C77312-4906-4A3F-A583-522D85B4793D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58B5277-BA69-4C53-A165-ACF7DEB4B546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="438" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25080" yWindow="-5055" windowWidth="13740" windowHeight="23640" tabRatio="438" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,20 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Defects!$B$1:$E$34</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$B$1:$F$69</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -89,19 +102,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Due -&gt; End in List pages</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>icon pack</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>created at -&gt; added</t>
+    <t>'created at' overwritten when modifying</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>'created at' overwritten when modifying</t>
+    <t>Due -&gt; Completed in List pages</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>created at -&gt; created</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -109,10 +122,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="42" formatCode="_-&quot;₩&quot;* #,##0_-;\-&quot;₩&quot;* #,##0_-;_-&quot;₩&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="yy&quot;-&quot;m&quot;-&quot;d;@"/>
-    <numFmt numFmtId="177" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -157,7 +169,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -194,40 +206,22 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -596,18 +590,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F165"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" style="18" customWidth="1"/>
-    <col min="2" max="2" width="59.21875" style="16" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="15" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="22" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" style="22" customWidth="1"/>
-    <col min="6" max="6" width="50.21875" style="14" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="59.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="16" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" style="16" customWidth="1"/>
+    <col min="6" max="6" width="50.21875" style="12" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -630,650 +624,736 @@
       </c>
     </row>
     <row r="2" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="12"/>
-      <c r="B2" s="19" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="21">
+      <c r="C2" s="3" t="str">
+        <f>IF(E2&lt;&gt;"", "✓", "")</f>
+        <v/>
+      </c>
+      <c r="D2" s="15">
         <v>45777</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="14"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="15"/>
-      <c r="B3" s="19" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="22">
+      <c r="C3" s="3" t="str">
+        <f t="shared" ref="C3:C34" si="0">IF(E3&lt;&gt;"", "✓", "")</f>
+        <v/>
+      </c>
+      <c r="D3" s="16">
         <v>45777</v>
       </c>
     </row>
     <row r="4" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="21">
+      <c r="C4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D4" s="15">
         <v>45777</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="14"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="15"/>
-      <c r="B5" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="22">
+      <c r="A5" s="8"/>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D5" s="16">
         <v>45777</v>
       </c>
     </row>
     <row r="6" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="21">
+      <c r="A6" s="3"/>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>✓</v>
+      </c>
+      <c r="D6" s="15">
         <v>45777</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="14"/>
+      <c r="E6" s="15">
+        <v>45777</v>
+      </c>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="14"/>
+      <c r="A7" s="3"/>
+      <c r="C7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="12"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="14"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="14"/>
+      <c r="A9" s="3"/>
+      <c r="C9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="14"/>
+      <c r="A10" s="3"/>
+      <c r="C10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="15"/>
+      <c r="A11" s="8"/>
+      <c r="C11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="12" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="14"/>
+      <c r="A12" s="3"/>
+      <c r="C12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="14"/>
+      <c r="A13" s="3"/>
+      <c r="C13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="14"/>
+      <c r="A14" s="3"/>
+      <c r="C14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="14"/>
+      <c r="A15" s="3"/>
+      <c r="C15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="14"/>
+      <c r="A16" s="3"/>
+      <c r="C16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="12"/>
     </row>
     <row r="17" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="15"/>
+      <c r="A17" s="8"/>
+      <c r="C17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="18" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="14"/>
+      <c r="A18" s="3"/>
+      <c r="C18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="14"/>
+      <c r="A19" s="3"/>
+      <c r="C19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="14"/>
+      <c r="A20" s="3"/>
+      <c r="C20" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="12"/>
     </row>
     <row r="21" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="14"/>
+      <c r="A21" s="3"/>
+      <c r="C21" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="12"/>
     </row>
     <row r="22" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="14"/>
+      <c r="A22" s="3"/>
+      <c r="C22" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="12"/>
     </row>
     <row r="23" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="15"/>
+      <c r="A23" s="8"/>
+      <c r="C23" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="24" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="12"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="14"/>
+      <c r="A24" s="3"/>
+      <c r="C24" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="12"/>
     </row>
     <row r="25" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="12"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="14"/>
+      <c r="A25" s="3"/>
+      <c r="C25" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="12"/>
     </row>
     <row r="26" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="12"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="14"/>
+      <c r="A26" s="3"/>
+      <c r="C26" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="12"/>
     </row>
     <row r="27" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="12"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="14"/>
+      <c r="A27" s="3"/>
+      <c r="C27" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="12"/>
     </row>
     <row r="28" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="12"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="14"/>
+      <c r="A28" s="3"/>
+      <c r="C28" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="12"/>
     </row>
     <row r="29" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="15"/>
+      <c r="A29" s="8"/>
+      <c r="C29" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="15"/>
+      <c r="A30" s="8"/>
+      <c r="C30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="31" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="12"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="14"/>
+      <c r="A31" s="3"/>
+      <c r="C31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="12"/>
     </row>
     <row r="32" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="12"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="14"/>
+      <c r="A32" s="3"/>
+      <c r="C32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="12"/>
     </row>
     <row r="33" spans="1:6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="12"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="14"/>
+      <c r="A33" s="3"/>
+      <c r="C33" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="12"/>
     </row>
     <row r="34" spans="1:6" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="12"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="14"/>
+      <c r="A34" s="3"/>
+      <c r="C34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="12"/>
     </row>
     <row r="35" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="15"/>
+      <c r="A35" s="8"/>
     </row>
     <row r="36" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="15"/>
+      <c r="A36" s="8"/>
     </row>
     <row r="37" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="15"/>
+      <c r="A37" s="8"/>
     </row>
     <row r="38" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="15"/>
+      <c r="A38" s="8"/>
     </row>
     <row r="39" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="15"/>
+      <c r="A39" s="8"/>
     </row>
     <row r="40" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="15"/>
+      <c r="A40" s="8"/>
     </row>
     <row r="41" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="15"/>
+      <c r="A41" s="8"/>
     </row>
     <row r="42" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="15"/>
+      <c r="A42" s="8"/>
     </row>
     <row r="43" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="15"/>
+      <c r="A43" s="8"/>
     </row>
     <row r="44" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="15"/>
+      <c r="A44" s="8"/>
     </row>
     <row r="45" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="15"/>
+      <c r="A45" s="8"/>
     </row>
     <row r="46" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="15"/>
+      <c r="A46" s="8"/>
     </row>
     <row r="47" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="15"/>
+      <c r="A47" s="8"/>
     </row>
     <row r="48" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="15"/>
+      <c r="A48" s="8"/>
     </row>
     <row r="49" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="15"/>
+      <c r="A49" s="8"/>
     </row>
     <row r="50" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="15"/>
+      <c r="A50" s="8"/>
     </row>
     <row r="51" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="15"/>
+      <c r="A51" s="8"/>
     </row>
     <row r="52" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="15"/>
+      <c r="A52" s="8"/>
     </row>
     <row r="53" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="15"/>
+      <c r="A53" s="8"/>
     </row>
     <row r="54" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="15"/>
+      <c r="A54" s="8"/>
     </row>
     <row r="55" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="15"/>
+      <c r="A55" s="8"/>
     </row>
     <row r="56" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="15"/>
+      <c r="A56" s="8"/>
     </row>
     <row r="57" spans="1:1" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="15"/>
+      <c r="A57" s="8"/>
     </row>
     <row r="58" spans="1:1" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="15"/>
+      <c r="A58" s="8"/>
     </row>
     <row r="59" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="15"/>
+      <c r="A59" s="8"/>
     </row>
     <row r="60" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="15"/>
+      <c r="A60" s="8"/>
     </row>
     <row r="61" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="15"/>
+      <c r="A61" s="8"/>
     </row>
     <row r="62" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="15"/>
+      <c r="A62" s="8"/>
     </row>
     <row r="63" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="15"/>
+      <c r="A63" s="8"/>
     </row>
     <row r="64" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="15"/>
+      <c r="A64" s="8"/>
     </row>
     <row r="65" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="15"/>
+      <c r="A65" s="8"/>
     </row>
     <row r="66" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="15"/>
+      <c r="A66" s="8"/>
     </row>
     <row r="67" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="15"/>
+      <c r="A67" s="8"/>
     </row>
     <row r="68" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="15"/>
+      <c r="A68" s="8"/>
     </row>
     <row r="69" spans="1:1" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="15"/>
+      <c r="A69" s="8"/>
     </row>
     <row r="70" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="15"/>
+      <c r="A70" s="8"/>
     </row>
     <row r="71" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="15"/>
+      <c r="A71" s="8"/>
     </row>
     <row r="72" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="15"/>
+      <c r="A72" s="8"/>
     </row>
     <row r="73" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="15"/>
+      <c r="A73" s="8"/>
     </row>
     <row r="74" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="15"/>
+      <c r="A74" s="8"/>
     </row>
     <row r="75" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A75" s="15"/>
+      <c r="A75" s="8"/>
     </row>
     <row r="76" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="15"/>
+      <c r="A76" s="8"/>
     </row>
     <row r="77" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="15"/>
+      <c r="A77" s="8"/>
     </row>
     <row r="78" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="15"/>
+      <c r="A78" s="8"/>
     </row>
     <row r="79" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="15"/>
+      <c r="A79" s="8"/>
     </row>
     <row r="80" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A80" s="15"/>
+      <c r="A80" s="8"/>
     </row>
     <row r="81" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A81" s="15"/>
+      <c r="A81" s="8"/>
     </row>
     <row r="82" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A82" s="15"/>
+      <c r="A82" s="8"/>
     </row>
     <row r="83" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="15"/>
+      <c r="A83" s="8"/>
     </row>
     <row r="84" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="15"/>
+      <c r="A84" s="8"/>
     </row>
     <row r="85" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="15"/>
+      <c r="A85" s="8"/>
     </row>
     <row r="86" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A86" s="15"/>
+      <c r="A86" s="8"/>
     </row>
     <row r="87" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A87" s="15"/>
+      <c r="A87" s="8"/>
     </row>
     <row r="88" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="15"/>
+      <c r="A88" s="8"/>
     </row>
     <row r="89" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A89" s="15"/>
+      <c r="A89" s="8"/>
     </row>
     <row r="90" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A90" s="15"/>
+      <c r="A90" s="8"/>
     </row>
     <row r="91" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A91" s="15"/>
+      <c r="A91" s="8"/>
     </row>
     <row r="92" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A92" s="15"/>
+      <c r="A92" s="8"/>
     </row>
     <row r="93" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="15"/>
+      <c r="A93" s="8"/>
     </row>
     <row r="94" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A94" s="15"/>
+      <c r="A94" s="8"/>
     </row>
     <row r="95" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A95" s="15"/>
+      <c r="A95" s="8"/>
     </row>
     <row r="96" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A96" s="15"/>
+      <c r="A96" s="8"/>
     </row>
     <row r="97" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A97" s="15"/>
+      <c r="A97" s="8"/>
     </row>
     <row r="98" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="15"/>
+      <c r="A98" s="8"/>
     </row>
     <row r="99" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A99" s="15"/>
+      <c r="A99" s="8"/>
     </row>
     <row r="100" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A100" s="15"/>
+      <c r="A100" s="8"/>
     </row>
     <row r="101" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A101" s="15"/>
+      <c r="A101" s="8"/>
     </row>
     <row r="102" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A102" s="15"/>
+      <c r="A102" s="8"/>
     </row>
     <row r="103" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="15"/>
+      <c r="A103" s="8"/>
     </row>
     <row r="104" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A104" s="15"/>
+      <c r="A104" s="8"/>
     </row>
     <row r="105" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A105" s="15"/>
+      <c r="A105" s="8"/>
     </row>
     <row r="106" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A106" s="15"/>
+      <c r="A106" s="8"/>
     </row>
     <row r="107" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A107" s="15"/>
+      <c r="A107" s="8"/>
     </row>
     <row r="108" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A108" s="15"/>
+      <c r="A108" s="8"/>
     </row>
     <row r="109" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A109" s="15"/>
+      <c r="A109" s="8"/>
     </row>
     <row r="110" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A110" s="15"/>
+      <c r="A110" s="8"/>
     </row>
     <row r="111" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A111" s="15"/>
+      <c r="A111" s="8"/>
     </row>
     <row r="112" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A112" s="15"/>
+      <c r="A112" s="8"/>
     </row>
     <row r="113" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A113" s="15"/>
+      <c r="A113" s="8"/>
     </row>
     <row r="114" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A114" s="15"/>
+      <c r="A114" s="8"/>
     </row>
     <row r="115" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A115" s="15"/>
+      <c r="A115" s="8"/>
     </row>
     <row r="116" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A116" s="15"/>
+      <c r="A116" s="8"/>
     </row>
     <row r="117" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A117" s="15"/>
+      <c r="A117" s="8"/>
     </row>
     <row r="118" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A118" s="15"/>
+      <c r="A118" s="8"/>
     </row>
     <row r="119" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A119" s="15"/>
+      <c r="A119" s="8"/>
     </row>
     <row r="120" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A120" s="15"/>
+      <c r="A120" s="8"/>
     </row>
     <row r="121" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A121" s="15"/>
+      <c r="A121" s="8"/>
     </row>
     <row r="122" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A122" s="15"/>
+      <c r="A122" s="8"/>
     </row>
     <row r="123" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A123" s="15"/>
+      <c r="A123" s="8"/>
     </row>
     <row r="124" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A124" s="15"/>
+      <c r="A124" s="8"/>
     </row>
     <row r="125" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A125" s="15"/>
+      <c r="A125" s="8"/>
     </row>
     <row r="126" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A126" s="15"/>
+      <c r="A126" s="8"/>
     </row>
     <row r="127" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A127" s="15"/>
+      <c r="A127" s="8"/>
     </row>
     <row r="128" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A128" s="15"/>
+      <c r="A128" s="8"/>
     </row>
     <row r="129" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A129" s="15"/>
+      <c r="A129" s="8"/>
     </row>
     <row r="130" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A130" s="15"/>
+      <c r="A130" s="8"/>
     </row>
     <row r="131" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A131" s="15"/>
+      <c r="A131" s="8"/>
     </row>
     <row r="132" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A132" s="15"/>
+      <c r="A132" s="8"/>
     </row>
     <row r="133" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A133" s="15"/>
+      <c r="A133" s="8"/>
     </row>
     <row r="134" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A134" s="15"/>
+      <c r="A134" s="8"/>
     </row>
     <row r="135" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A135" s="15"/>
+      <c r="A135" s="8"/>
     </row>
     <row r="136" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A136" s="15"/>
+      <c r="A136" s="8"/>
     </row>
     <row r="137" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A137" s="15"/>
+      <c r="A137" s="8"/>
     </row>
     <row r="138" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A138" s="15"/>
+      <c r="A138" s="8"/>
     </row>
     <row r="139" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A139" s="15"/>
+      <c r="A139" s="8"/>
     </row>
     <row r="140" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A140" s="15"/>
+      <c r="A140" s="8"/>
     </row>
     <row r="141" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A141" s="15"/>
+      <c r="A141" s="8"/>
     </row>
     <row r="142" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A142" s="15"/>
+      <c r="A142" s="8"/>
     </row>
     <row r="143" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A143" s="15"/>
+      <c r="A143" s="8"/>
     </row>
     <row r="144" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A144" s="15"/>
+      <c r="A144" s="8"/>
     </row>
     <row r="145" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A145" s="15"/>
+      <c r="A145" s="8"/>
     </row>
     <row r="146" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A146" s="15"/>
+      <c r="A146" s="8"/>
     </row>
     <row r="147" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A147" s="15"/>
+      <c r="A147" s="8"/>
     </row>
     <row r="148" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A148" s="15"/>
+      <c r="A148" s="8"/>
     </row>
     <row r="149" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A149" s="15"/>
+      <c r="A149" s="8"/>
     </row>
     <row r="150" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A150" s="15"/>
+      <c r="A150" s="8"/>
     </row>
     <row r="151" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A151" s="15"/>
+      <c r="A151" s="8"/>
     </row>
     <row r="152" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A152" s="15"/>
+      <c r="A152" s="8"/>
     </row>
     <row r="153" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A153" s="15"/>
+      <c r="A153" s="8"/>
     </row>
     <row r="154" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A154" s="15"/>
+      <c r="A154" s="8"/>
     </row>
     <row r="155" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A155" s="15"/>
+      <c r="A155" s="8"/>
     </row>
     <row r="156" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A156" s="15"/>
+      <c r="A156" s="8"/>
     </row>
     <row r="157" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A157" s="15"/>
+      <c r="A157" s="8"/>
     </row>
     <row r="158" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A158" s="15"/>
+      <c r="A158" s="8"/>
     </row>
     <row r="159" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A159" s="15"/>
+      <c r="A159" s="8"/>
     </row>
     <row r="160" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A160" s="15"/>
+      <c r="A160" s="8"/>
     </row>
     <row r="161" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A161" s="15"/>
+      <c r="A161" s="8"/>
     </row>
     <row r="162" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A162" s="15"/>
+      <c r="A162" s="8"/>
     </row>
     <row r="163" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A163" s="15"/>
+      <c r="A163" s="8"/>
     </row>
     <row r="164" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A164" s="15"/>
+      <c r="A164" s="8"/>
     </row>
     <row r="165" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A165" s="15"/>
+      <c r="A165" s="8"/>
     </row>
   </sheetData>
   <autoFilter ref="B1:F69" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
@@ -1288,18 +1368,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F167"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="59.21875" style="16" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="15" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="22" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" style="22" customWidth="1"/>
-    <col min="6" max="6" width="50.21875" style="14" customWidth="1"/>
+    <col min="1" max="1" width="1.6640625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="59.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="16" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" style="16" customWidth="1"/>
+    <col min="6" max="6" width="50.21875" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1321,616 +1401,783 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="21">
+      <c r="A2" s="3"/>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="3" t="str">
+        <f>IF(E2&lt;&gt;"", "✓", "")</f>
+        <v>✓</v>
+      </c>
+      <c r="D2" s="15">
         <v>45777</v>
       </c>
-      <c r="E2" s="21"/>
+      <c r="E2" s="15">
+        <v>45777</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="12"/>
-      <c r="B3" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="21">
+      <c r="A3" s="3"/>
+      <c r="B3" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="str">
+        <f t="shared" ref="C3:C49" si="0">IF(E3&lt;&gt;"", "✓", "")</f>
+        <v/>
+      </c>
+      <c r="D3" s="15">
         <v>45777</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
+      <c r="A4" s="3"/>
+      <c r="B4"/>
+      <c r="C4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
     </row>
     <row r="5" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="12"/>
+      <c r="A5" s="3"/>
+      <c r="C5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="A6" s="3"/>
+      <c r="B6"/>
+      <c r="C6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
     </row>
     <row r="7" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="A7" s="3"/>
+      <c r="B7"/>
+      <c r="C7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
     </row>
     <row r="8" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
+      <c r="A8" s="3"/>
+      <c r="C8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
     </row>
     <row r="9" spans="1:6" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
+      <c r="A9" s="3"/>
+      <c r="B9"/>
+      <c r="C9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
     </row>
     <row r="10" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
+      <c r="A10" s="3"/>
+      <c r="B10"/>
+      <c r="C10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
     </row>
     <row r="11" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="12"/>
+      <c r="A11" s="3"/>
+      <c r="C11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
+      <c r="A12" s="3"/>
+      <c r="B12"/>
+      <c r="C12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
     </row>
     <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
+      <c r="A13" s="3"/>
+      <c r="B13"/>
+      <c r="C13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
+      <c r="A14" s="3"/>
+      <c r="B14"/>
+      <c r="C14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
     </row>
     <row r="15" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
+      <c r="A15" s="3"/>
+      <c r="B15"/>
+      <c r="C15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
     </row>
     <row r="16" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
+      <c r="A16" s="3"/>
+      <c r="B16"/>
+      <c r="C16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
     </row>
     <row r="17" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="12"/>
+      <c r="A17" s="3"/>
+      <c r="C17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
+      <c r="A18" s="3"/>
+      <c r="B18"/>
+      <c r="C18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
     </row>
     <row r="19" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
+      <c r="A19" s="3"/>
+      <c r="B19"/>
+      <c r="C19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
     </row>
     <row r="20" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
+      <c r="A20" s="3"/>
+      <c r="B20"/>
+      <c r="C20" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
     </row>
     <row r="21" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
+      <c r="A21" s="3"/>
+      <c r="B21"/>
+      <c r="C21" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
     </row>
     <row r="22" spans="1:5" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
+      <c r="A22" s="3"/>
+      <c r="B22"/>
+      <c r="C22" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
     </row>
     <row r="23" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="12"/>
+      <c r="A23" s="3"/>
+      <c r="C23" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="12"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
+      <c r="A24" s="3"/>
+      <c r="B24"/>
+      <c r="C24" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
     </row>
     <row r="25" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="12"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
+      <c r="A25" s="3"/>
+      <c r="B25"/>
+      <c r="C25" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
     </row>
     <row r="26" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="12"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
+      <c r="A26" s="3"/>
+      <c r="B26"/>
+      <c r="C26" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
     </row>
     <row r="27" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="12"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
+      <c r="A27" s="3"/>
+      <c r="B27"/>
+      <c r="C27" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
     </row>
     <row r="28" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="12"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
+      <c r="A28" s="3"/>
+      <c r="B28"/>
+      <c r="C28" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
     </row>
     <row r="29" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="12"/>
+      <c r="A29" s="3"/>
+      <c r="C29" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="30" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="12"/>
+      <c r="A30" s="3"/>
+      <c r="C30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="12"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
+      <c r="A31" s="3"/>
+      <c r="B31"/>
+      <c r="C31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
     </row>
     <row r="32" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="12"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
+      <c r="A32" s="3"/>
+      <c r="B32"/>
+      <c r="C32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
     </row>
     <row r="33" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="12"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
+      <c r="A33" s="3"/>
+      <c r="B33"/>
+      <c r="C33" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
     </row>
     <row r="34" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="12"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
+      <c r="A34" s="3"/>
+      <c r="B34"/>
+      <c r="C34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
     </row>
     <row r="35" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="12"/>
+      <c r="A35" s="3"/>
+      <c r="C35" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="36" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="12"/>
+      <c r="A36" s="3"/>
+      <c r="C36" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="37" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="12"/>
+      <c r="A37" s="3"/>
+      <c r="C37" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="38" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="12"/>
+      <c r="A38" s="3"/>
+      <c r="C38" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="39" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="12"/>
+      <c r="A39" s="3"/>
+      <c r="C39" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="40" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="12"/>
+      <c r="A40" s="3"/>
+      <c r="C40" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="41" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="12"/>
+      <c r="A41" s="3"/>
+      <c r="C41" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="42" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="12"/>
+      <c r="A42" s="3"/>
+      <c r="C42" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="43" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="12"/>
+      <c r="A43" s="3"/>
+      <c r="C43" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="44" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="12"/>
+      <c r="A44" s="3"/>
+      <c r="C44" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="45" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="12"/>
+      <c r="A45" s="3"/>
+      <c r="C45" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="46" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="12"/>
+      <c r="A46" s="3"/>
+      <c r="C46" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="47" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="12"/>
+      <c r="A47" s="3"/>
+      <c r="C47" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="48" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="12"/>
-    </row>
-    <row r="49" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="12"/>
-    </row>
-    <row r="50" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="12"/>
-    </row>
-    <row r="51" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="12"/>
-    </row>
-    <row r="52" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="12"/>
-    </row>
-    <row r="53" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="12"/>
-    </row>
-    <row r="54" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="12"/>
-    </row>
-    <row r="55" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="12"/>
-    </row>
-    <row r="56" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="12"/>
-    </row>
-    <row r="57" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="12"/>
-    </row>
-    <row r="58" spans="1:1" ht="13.5" x14ac:dyDescent="0.15">
-      <c r="A58" s="12"/>
-    </row>
-    <row r="59" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="12"/>
-    </row>
-    <row r="60" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="12"/>
-    </row>
-    <row r="61" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="12"/>
-    </row>
-    <row r="62" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="12"/>
-    </row>
-    <row r="63" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="12"/>
-    </row>
-    <row r="64" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="12"/>
+      <c r="A48" s="3"/>
+      <c r="C48" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="3"/>
+      <c r="C49" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="3"/>
+    </row>
+    <row r="51" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="3"/>
+    </row>
+    <row r="52" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="3"/>
+    </row>
+    <row r="53" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="3"/>
+    </row>
+    <row r="54" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="3"/>
+    </row>
+    <row r="55" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="3"/>
+    </row>
+    <row r="56" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="3"/>
+    </row>
+    <row r="57" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="3"/>
+    </row>
+    <row r="58" spans="1:3" ht="13.5" x14ac:dyDescent="0.15">
+      <c r="A58" s="3"/>
+    </row>
+    <row r="59" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="3"/>
+    </row>
+    <row r="60" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="3"/>
+    </row>
+    <row r="61" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A61" s="3"/>
+    </row>
+    <row r="62" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A62" s="3"/>
+    </row>
+    <row r="63" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="3"/>
+    </row>
+    <row r="64" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A64" s="3"/>
     </row>
     <row r="65" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="12"/>
+      <c r="A65" s="3"/>
     </row>
     <row r="66" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="12"/>
+      <c r="A66" s="3"/>
     </row>
     <row r="67" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="12"/>
+      <c r="A67" s="3"/>
     </row>
     <row r="68" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="12"/>
+      <c r="A68" s="3"/>
     </row>
     <row r="69" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="12"/>
+      <c r="A69" s="3"/>
     </row>
     <row r="70" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="12"/>
+      <c r="A70" s="3"/>
     </row>
     <row r="71" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="12"/>
+      <c r="A71" s="3"/>
     </row>
     <row r="72" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="12"/>
+      <c r="A72" s="3"/>
     </row>
     <row r="73" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="12"/>
+      <c r="A73" s="3"/>
     </row>
     <row r="74" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="12"/>
+      <c r="A74" s="3"/>
     </row>
     <row r="75" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A75" s="12"/>
+      <c r="A75" s="3"/>
     </row>
     <row r="76" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="12"/>
+      <c r="A76" s="3"/>
     </row>
     <row r="77" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="12"/>
+      <c r="A77" s="3"/>
     </row>
     <row r="78" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="12"/>
+      <c r="A78" s="3"/>
     </row>
     <row r="79" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="12"/>
+      <c r="A79" s="3"/>
     </row>
     <row r="80" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A80" s="12"/>
+      <c r="A80" s="3"/>
     </row>
     <row r="81" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A81" s="12"/>
+      <c r="A81" s="3"/>
     </row>
     <row r="82" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A82" s="12"/>
+      <c r="A82" s="3"/>
     </row>
     <row r="83" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="12"/>
+      <c r="A83" s="3"/>
     </row>
     <row r="84" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="12"/>
+      <c r="A84" s="3"/>
     </row>
     <row r="85" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="12"/>
+      <c r="A85" s="3"/>
     </row>
     <row r="86" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A86" s="12"/>
+      <c r="A86" s="3"/>
     </row>
     <row r="87" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A87" s="12"/>
+      <c r="A87" s="3"/>
     </row>
     <row r="88" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="12"/>
+      <c r="A88" s="3"/>
     </row>
     <row r="89" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A89" s="12"/>
+      <c r="A89" s="3"/>
     </row>
     <row r="90" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A90" s="12"/>
+      <c r="A90" s="3"/>
     </row>
     <row r="91" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A91" s="12"/>
+      <c r="A91" s="3"/>
     </row>
     <row r="92" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A92" s="12"/>
+      <c r="A92" s="3"/>
     </row>
     <row r="93" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="12"/>
+      <c r="A93" s="3"/>
     </row>
     <row r="94" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A94" s="12"/>
+      <c r="A94" s="3"/>
     </row>
     <row r="95" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A95" s="12"/>
+      <c r="A95" s="3"/>
     </row>
     <row r="96" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A96" s="12"/>
+      <c r="A96" s="3"/>
     </row>
     <row r="97" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A97" s="12"/>
+      <c r="A97" s="3"/>
     </row>
     <row r="98" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="12"/>
+      <c r="A98" s="3"/>
     </row>
     <row r="99" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A99" s="12"/>
+      <c r="A99" s="3"/>
     </row>
     <row r="100" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A100" s="12"/>
+      <c r="A100" s="3"/>
     </row>
     <row r="101" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A101" s="12"/>
+      <c r="A101" s="3"/>
     </row>
     <row r="102" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A102" s="12"/>
+      <c r="A102" s="3"/>
     </row>
     <row r="103" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="12"/>
+      <c r="A103" s="3"/>
     </row>
     <row r="104" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A104" s="12"/>
+      <c r="A104" s="3"/>
     </row>
     <row r="105" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A105" s="12"/>
+      <c r="A105" s="3"/>
     </row>
     <row r="106" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A106" s="12"/>
+      <c r="A106" s="3"/>
     </row>
     <row r="107" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A107" s="12"/>
+      <c r="A107" s="3"/>
     </row>
     <row r="108" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A108" s="12"/>
+      <c r="A108" s="3"/>
     </row>
     <row r="109" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A109" s="12"/>
+      <c r="A109" s="3"/>
     </row>
     <row r="110" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A110" s="12"/>
+      <c r="A110" s="3"/>
     </row>
     <row r="111" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A111" s="12"/>
+      <c r="A111" s="3"/>
     </row>
     <row r="112" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A112" s="12"/>
+      <c r="A112" s="3"/>
     </row>
     <row r="113" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A113" s="12"/>
+      <c r="A113" s="3"/>
     </row>
     <row r="114" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A114" s="12"/>
+      <c r="A114" s="3"/>
     </row>
     <row r="115" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A115" s="12"/>
+      <c r="A115" s="3"/>
     </row>
     <row r="116" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A116" s="12"/>
+      <c r="A116" s="3"/>
     </row>
     <row r="117" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A117" s="12"/>
+      <c r="A117" s="3"/>
     </row>
     <row r="118" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A118" s="12"/>
+      <c r="A118" s="3"/>
     </row>
     <row r="119" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A119" s="12"/>
+      <c r="A119" s="3"/>
     </row>
     <row r="120" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A120" s="12"/>
+      <c r="A120" s="3"/>
     </row>
     <row r="121" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A121" s="12"/>
+      <c r="A121" s="3"/>
     </row>
     <row r="122" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A122" s="12"/>
+      <c r="A122" s="3"/>
     </row>
     <row r="123" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A123" s="12"/>
+      <c r="A123" s="3"/>
     </row>
     <row r="124" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A124" s="12"/>
+      <c r="A124" s="3"/>
     </row>
     <row r="125" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A125" s="12"/>
+      <c r="A125" s="3"/>
     </row>
     <row r="126" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A126" s="12"/>
+      <c r="A126" s="3"/>
     </row>
     <row r="127" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A127" s="12"/>
+      <c r="A127" s="3"/>
     </row>
     <row r="128" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A128" s="12"/>
+      <c r="A128" s="3"/>
     </row>
     <row r="129" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A129" s="12"/>
+      <c r="A129" s="3"/>
     </row>
     <row r="130" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A130" s="12"/>
+      <c r="A130" s="3"/>
     </row>
     <row r="131" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A131" s="12"/>
+      <c r="A131" s="3"/>
     </row>
     <row r="132" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A132" s="12"/>
+      <c r="A132" s="3"/>
     </row>
     <row r="133" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A133" s="12"/>
+      <c r="A133" s="3"/>
     </row>
     <row r="134" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A134" s="12"/>
+      <c r="A134" s="3"/>
     </row>
     <row r="135" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A135" s="12"/>
+      <c r="A135" s="3"/>
     </row>
     <row r="136" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A136" s="12"/>
+      <c r="A136" s="3"/>
     </row>
     <row r="137" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A137" s="12"/>
+      <c r="A137" s="3"/>
     </row>
     <row r="138" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A138" s="12"/>
+      <c r="A138" s="3"/>
     </row>
     <row r="139" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A139" s="12"/>
+      <c r="A139" s="3"/>
     </row>
     <row r="140" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A140" s="12"/>
+      <c r="A140" s="3"/>
     </row>
     <row r="141" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A141" s="12"/>
+      <c r="A141" s="3"/>
     </row>
     <row r="142" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A142" s="12"/>
+      <c r="A142" s="3"/>
     </row>
     <row r="143" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A143" s="12"/>
+      <c r="A143" s="3"/>
     </row>
     <row r="144" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A144" s="12"/>
+      <c r="A144" s="3"/>
     </row>
     <row r="145" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A145" s="12"/>
+      <c r="A145" s="3"/>
     </row>
     <row r="146" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A146" s="12"/>
+      <c r="A146" s="3"/>
     </row>
     <row r="147" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A147" s="12"/>
+      <c r="A147" s="3"/>
     </row>
     <row r="148" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A148" s="12"/>
+      <c r="A148" s="3"/>
     </row>
     <row r="149" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A149" s="12"/>
+      <c r="A149" s="3"/>
     </row>
     <row r="150" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A150" s="12"/>
+      <c r="A150" s="3"/>
     </row>
     <row r="151" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A151" s="12"/>
+      <c r="A151" s="3"/>
     </row>
     <row r="152" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A152" s="12"/>
+      <c r="A152" s="3"/>
     </row>
     <row r="153" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A153" s="12"/>
+      <c r="A153" s="3"/>
     </row>
     <row r="154" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A154" s="12"/>
+      <c r="A154" s="3"/>
     </row>
     <row r="155" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A155" s="12"/>
+      <c r="A155" s="3"/>
     </row>
     <row r="156" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A156" s="12"/>
+      <c r="A156" s="3"/>
     </row>
     <row r="157" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A157" s="12"/>
+      <c r="A157" s="3"/>
     </row>
     <row r="158" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A158" s="12"/>
+      <c r="A158" s="3"/>
     </row>
     <row r="159" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A159" s="12"/>
+      <c r="A159" s="3"/>
     </row>
     <row r="160" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A160" s="12"/>
+      <c r="A160" s="3"/>
     </row>
     <row r="161" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A161" s="12"/>
+      <c r="A161" s="3"/>
     </row>
     <row r="162" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A162" s="12"/>
+      <c r="A162" s="3"/>
     </row>
     <row r="163" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A163" s="12"/>
+      <c r="A163" s="3"/>
     </row>
     <row r="164" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A164" s="12"/>
+      <c r="A164" s="3"/>
     </row>
     <row r="165" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A165" s="12"/>
+      <c r="A165" s="3"/>
     </row>
     <row r="166" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A166" s="12"/>
+      <c r="A166" s="3"/>
     </row>
     <row r="167" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A167" s="12"/>
+      <c r="A167" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="B1:E34" xr:uid="{00000000-0009-0000-0000-000001000000}"/>

</xml_diff>

<commit_message>
fix: 'created at' overwritten when modifying
</commit_message>
<xml_diff>
--- a/doc/tasks.xlsx
+++ b/doc/tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\git\web\plan-it\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58B5277-BA69-4C53-A165-ACF7DEB4B546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5367F7C6-FE67-4B5A-A61B-E4A049296AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-5055" windowWidth="13740" windowHeight="23640" tabRatio="438" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25080" yWindow="-5055" windowWidth="13740" windowHeight="23640" tabRatio="438" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Task</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -115,6 +115,10 @@
   </si>
   <si>
     <t>created at -&gt; created</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enhance recent list ui</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -590,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -698,11 +702,16 @@
     </row>
     <row r="7" spans="1:6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3"/>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
       <c r="C7" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D7" s="15"/>
+      <c r="D7" s="15">
+        <v>45777</v>
+      </c>
       <c r="E7" s="15"/>
       <c r="F7" s="12"/>
     </row>
@@ -1368,8 +1377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F167"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1423,9 +1432,12 @@
       </c>
       <c r="C3" s="3" t="str">
         <f t="shared" ref="C3:C49" si="0">IF(E3&lt;&gt;"", "✓", "")</f>
-        <v/>
+        <v>✓</v>
       </c>
       <c r="D3" s="15">
+        <v>45777</v>
+      </c>
+      <c r="E3" s="16">
         <v>45777</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Apply new Recent List design to Dashboard
</commit_message>
<xml_diff>
--- a/doc/tasks.xlsx
+++ b/doc/tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\git\web\plan-it\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD42654-3A4C-49B9-B005-03C689761531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17235C1-B0C4-462D-8A89-4D9991CDD2DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-5055" windowWidth="13740" windowHeight="23640" tabRatio="438" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25080" yWindow="3450" windowWidth="13500" windowHeight="14790" tabRatio="438" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -602,7 +602,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -717,12 +719,14 @@
       </c>
       <c r="C7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>✓</v>
       </c>
       <c r="D7" s="15">
         <v>45777</v>
       </c>
-      <c r="E7" s="15"/>
+      <c r="E7" s="15">
+        <v>45778</v>
+      </c>
       <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
fix: NaN% shown when no tasks on Dashboard
</commit_message>
<xml_diff>
--- a/doc/tasks.xlsx
+++ b/doc/tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\git\web\plan-it\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17235C1-B0C4-462D-8A89-4D9991CDD2DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486237CF-F4A4-40D1-9392-0E131EA9A638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="3450" windowWidth="13500" windowHeight="14790" tabRatio="438" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25080" yWindow="-5055" windowWidth="13740" windowHeight="23640" tabRatio="438" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Task</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -127,6 +127,10 @@
   </si>
   <si>
     <t>later, need apply icon pack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NaN% shown when no tasks on Dashboard</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -602,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1395,8 +1399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F167"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1461,13 +1465,19 @@
     </row>
     <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3"/>
-      <c r="B4"/>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
       <c r="C4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
+        <v>✓</v>
+      </c>
+      <c r="D4" s="15">
+        <v>45778</v>
+      </c>
+      <c r="E4" s="15">
+        <v>45779</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3"/>

</xml_diff>

<commit_message>
complete conversion to tailwind
</commit_message>
<xml_diff>
--- a/doc/tasks.xlsx
+++ b/doc/tasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\git\web\plan-it\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA9E415-C982-42D2-99FF-000952AB5F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BC65C7-08E9-48C7-9B37-EA2648B6AD4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-5055" windowWidth="13740" windowHeight="23640" tabRatio="438" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="438" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -615,7 +615,7 @@
   <dimension ref="A1:F165"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -654,12 +654,14 @@
       </c>
       <c r="C2" s="3" t="str">
         <f>IF(E2&lt;&gt;"", "✓", "")</f>
-        <v/>
+        <v>✓</v>
       </c>
       <c r="D2" s="15">
         <v>45777</v>
       </c>
-      <c r="E2" s="15"/>
+      <c r="E2" s="15">
+        <v>45789</v>
+      </c>
       <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>